<commit_message>
database changes and mail robot
</commit_message>
<xml_diff>
--- a/Excel/Email Hustle.xlsx
+++ b/Excel/Email Hustle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\gbilton\Personal\sampa-back\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9577DE-96F6-46B3-A661-10759DD15298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3202CDF-B640-494B-B8A4-55770CEA13F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3291,9 +3291,9 @@
   </sheetPr>
   <dimension ref="A1:AC968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>

</xml_diff>